<commit_message>
removed all generated files
</commit_message>
<xml_diff>
--- a/21xt/03-wireless_strain_gauge/wsg1.0/NewBOM.xlsx
+++ b/21xt/03-wireless_strain_gauge/wsg1.0/NewBOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahmoudradwan/Desktop/bjr_kicad/21xt/03-wireless_strain_gauge/wsg1.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363699FC-6406-4A42-8B52-2BE3550E361C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5384D0A-A5E0-3E44-93E0-EB25A59781FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="800" windowWidth="27640" windowHeight="15900" xr2:uid="{CF41C47E-5475-C94D-83CE-C556D60A32D0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{CF41C47E-5475-C94D-83CE-C556D60A32D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>Id</t>
   </si>
@@ -68,18 +68,12 @@
     <t>C23182</t>
   </si>
   <si>
-    <t>47u</t>
-  </si>
-  <si>
     <t>47uF</t>
   </si>
   <si>
     <t>C178330</t>
   </si>
   <si>
-    <t>22u</t>
-  </si>
-  <si>
     <t>22uF</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
     <t>C14663</t>
   </si>
   <si>
-    <t>LinRef1,LinReg2,LinReg3</t>
-  </si>
-  <si>
     <t>SOT91P240X110-3N</t>
   </si>
   <si>
@@ -170,17 +161,38 @@
     <t>C153761</t>
   </si>
   <si>
-    <t>Add to BOM</t>
-  </si>
-  <si>
-    <t>yes</t>
+    <t>C12,C10,C14,C8,C4</t>
+  </si>
+  <si>
+    <t>100uF</t>
+  </si>
+  <si>
+    <t>C19702</t>
+  </si>
+  <si>
+    <t>C20346010</t>
+  </si>
+  <si>
+    <t>BConv1</t>
+  </si>
+  <si>
+    <t>TPSM83100SIUR</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>LinReg1,LinReg2,LinReg3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -195,20 +207,27 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF222222"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF409EFF"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF666666"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -234,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -242,13 +261,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,15 +587,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6ED14B0-FE9C-9D41-8E28-041425D4CDF2}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -590,11 +620,9 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -610,19 +638,16 @@
       <c r="E2" s="2">
         <v>47</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -631,21 +656,18 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -654,21 +676,18 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -677,67 +696,60 @@
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2">
         <v>3</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -746,106 +758,149 @@
         <v>2</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="2" t="s">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="2:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="G23" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>